<commit_message>
KIBON-1664 add keinSelbstbehaltDurchGemeinde Flag to LastenausgleichSelbstbehalt.xlsx to verify Lastenausgleich
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichSelbstbehalt.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichSelbstbehalt.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74DC510-6DC7-47CC-97DA-D6D8086D7F42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB9312-69FA-49A5-9EC4-63F0A62ADB01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="anteil">Data!$R$8</definedName>
-    <definedName name="gutschein">Data!$L$8</definedName>
+    <definedName name="anteil">Data!$T$8</definedName>
+    <definedName name="anteilOhneAsyl">Data!$U$8</definedName>
+    <definedName name="anzeilOhneAsyl">Data!$U$8</definedName>
+    <definedName name="gutschein">Data!$M$8</definedName>
+    <definedName name="gutscheinBetragOhneAsyl">Data!$N$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Lastenausgleich - Berechnung Selbstbehalt pro 100% Platz</t>
   </si>
@@ -146,6 +152,18 @@
   </si>
   <si>
     <t>{jahr}</t>
+  </si>
+  <si>
+    <t>Kein Selbstbehalt durch Gemeinde</t>
+  </si>
+  <si>
+    <t>Anteil Kalenderjahr (ohne Kinder mit ZEMIS Nummer)</t>
+  </si>
+  <si>
+    <t>{keinSelbstbehaltDurchGemeinde}</t>
+  </si>
+  <si>
+    <t>Gutscheinbetrag (ohne Kinder mit ZEMIS Nummer)</t>
   </si>
 </sst>
 </file>
@@ -153,7 +171,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$CHF-807]\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$CHF-807]\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -253,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -288,6 +306,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -300,22 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,7 +651,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFD2C01-3190-4613-9E97-C1D328FAAE82}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -645,28 +666,29 @@
     <col min="8" max="8" width="25.140625" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" customWidth="1"/>
+    <col min="13" max="14" width="26.28515625" customWidth="1"/>
     <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="18" width="20.85546875" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="20" width="20.85546875" customWidth="1"/>
+    <col min="21" max="21" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -674,83 +696,95 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="N6" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="P6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="Q6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="R6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="S6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="20" t="s">
+      <c r="T6" s="21" t="s">
         <v>33</v>
       </c>
+      <c r="U6" s="21" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="21"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -784,38 +818,49 @@
       <c r="K8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="4" t="e">
+      <c r="N8" s="16" t="str">
+        <f>IF(L8&lt;&gt;"X",M8,"")</f>
+        <v>{gutschein}</v>
+      </c>
+      <c r="O8" s="4" t="e">
         <f>E8-DAY(E8)+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N8" s="4" t="e">
-        <f t="shared" ref="N8" si="0">EOMONTH(E8,0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O8" s="11" t="e">
-        <f>N8-M8+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P8" s="11" t="e">
+      <c r="P8" s="4" t="e">
+        <f t="shared" ref="P8" si="0">EOMONTH(E8,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q8" s="11" t="e">
+        <f>P8-O8+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="11" t="e">
         <f>F8-E8+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q8" s="8" t="e">
-        <f>P8/O8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R8" s="12" t="e">
-        <f>G8*Q8/12</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="S8" s="8" t="e">
+        <f>R8/Q8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T8" s="12" t="e">
+        <f>G8*S8/12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U8" s="12" t="e">
+        <f>IF(L8&lt;&gt;"X",T8,"")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="9"/>
       <c r="C9" s="6"/>
@@ -827,61 +872,74 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="23">
+      <c r="L9" s="13"/>
+      <c r="M9" s="17">
         <f>SUM(gutschein)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="17">
+        <f>SUM(gutscheinBetragOhneAsyl)</f>
+        <v>0</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="13" t="e">
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="13" t="e">
         <f>SUM(anteil)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="U9" s="13" t="e">
+        <f>SUM(anteilOhneAsyl)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L10" s="25"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="24" t="e">
-        <f>L9/R9</f>
+      <c r="C11" s="20" t="e">
+        <f>N9/U9</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="24" t="e">
+      <c r="C12" s="18" t="e">
         <f>C11*0.2</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="G6:G7"/>
+  <mergeCells count="21">
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>